<commit_message>
Cleaned Up Docker and Kubernetes Notes
</commit_message>
<xml_diff>
--- a/kubernetes/Kubernetes-API-Objects.xlsx
+++ b/kubernetes/Kubernetes-API-Objects.xlsx
@@ -8,15 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\dssg\Distributed-Systems-Study-Group\kubernetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80B73B2-516F-4ACA-8765-2910DF964F94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF417F84-3742-4593-BC16-B0D4DA9365CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9709F4E-DB8A-44C0-BA47-BF5BE7E9CD0A}"/>
+    <workbookView xWindow="6108" yWindow="3744" windowWidth="17280" windowHeight="8964" xr2:uid="{C9709F4E-DB8A-44C0-BA47-BF5BE7E9CD0A}"/>
+    <workbookView xWindow="6456" yWindow="4092" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{DC345DA8-84C6-4CD2-BFD8-497499F40304}"/>
   </bookViews>
   <sheets>
-    <sheet name="1.16" sheetId="7" r:id="rId1"/>
+    <sheet name="1.17" sheetId="8" r:id="rId1"/>
+    <sheet name="1.16" sheetId="7" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1.16'!$A$1:$I$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1.16'!$A$1:$I$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1.17'!$A$1:$I$54</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="255" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="172">
   <si>
     <t>NAME</t>
   </si>
@@ -520,6 +525,36 @@
   </si>
   <si>
     <t>Deprecated</t>
+  </si>
+  <si>
+    <t>EndpointSlice</t>
+  </si>
+  <si>
+    <t>VolumeSnapshotClass</t>
+  </si>
+  <si>
+    <t>VolumeSnapshotContent</t>
+  </si>
+  <si>
+    <t>VolumeSnapshot</t>
+  </si>
+  <si>
+    <t>endpointslices</t>
+  </si>
+  <si>
+    <t>discovery.k8s.io</t>
+  </si>
+  <si>
+    <t>volumesnapshotclasses</t>
+  </si>
+  <si>
+    <t>snapshot.storage.k8s.io</t>
+  </si>
+  <si>
+    <t>volumesnapshotcontents</t>
+  </si>
+  <si>
+    <t>volumesnapshots</t>
   </si>
 </sst>
 </file>
@@ -883,13 +918,1027 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{813740EA-F19B-44C7-B395-629D3A4324F4}">
+  <dimension ref="A1:I57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A52:A57"/>
+    </sheetView>
+    <sheetView workbookViewId="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="I1" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F8" t="s">
+        <v>81</v>
+      </c>
+      <c r="G8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F9" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F12" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F15" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>158</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G17" s="1"/>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F19" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F21" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B22" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F22" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G24" s="1"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F25" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="1"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F26" t="s">
+        <v>47</v>
+      </c>
+      <c r="G26" s="1"/>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" t="s">
+        <v>49</v>
+      </c>
+      <c r="G27" s="1"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B28" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B29" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B30" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F30" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F31" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B32" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B33" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F34" t="s">
+        <v>56</v>
+      </c>
+      <c r="G34" s="1"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F35" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="1"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B36" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B37" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F37" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>153</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F38" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F39" t="s">
+        <v>13</v>
+      </c>
+      <c r="G39" s="1"/>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F40" t="s">
+        <v>62</v>
+      </c>
+      <c r="G40" s="1"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>153</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F41" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>153</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C42" t="s">
+        <v>64</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F42" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B43" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E43" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F43" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B44" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C45" t="s">
+        <v>134</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F45" t="s">
+        <v>109</v>
+      </c>
+      <c r="G45" s="1"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F46" t="s">
+        <v>111</v>
+      </c>
+      <c r="G46" s="1"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F47" t="s">
+        <v>112</v>
+      </c>
+      <c r="G47" s="1"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" t="s">
+        <v>71</v>
+      </c>
+      <c r="G48" s="1"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C49" s="1"/>
+      <c r="D49" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F49" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="1"/>
+      <c r="B50" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C50" t="s">
+        <v>114</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F50" t="s">
+        <v>116</v>
+      </c>
+      <c r="G50" s="1"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F51" t="s">
+        <v>163</v>
+      </c>
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="F52" t="s">
+        <v>164</v>
+      </c>
+      <c r="G52" s="1"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="F53" t="s">
+        <v>165</v>
+      </c>
+      <c r="G53" s="1"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" t="s">
+        <v>117</v>
+      </c>
+      <c r="E54" t="b">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B55" t="s">
+        <v>145</v>
+      </c>
+      <c r="D55" t="s">
+        <v>117</v>
+      </c>
+      <c r="E55" t="b">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B56" t="s">
+        <v>137</v>
+      </c>
+      <c r="C56" t="s">
+        <v>136</v>
+      </c>
+      <c r="D56" t="s">
+        <v>117</v>
+      </c>
+      <c r="E56" t="b">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B57" t="s">
+        <v>142</v>
+      </c>
+      <c r="D57" t="s">
+        <v>117</v>
+      </c>
+      <c r="E57" t="b">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>119</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{227E03F6-A8BF-43CC-A2FF-E71F0F26FEB8}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -922,7 +1971,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -933,7 +1982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B3" s="1" t="s">
         <v>76</v>
       </c>
@@ -947,7 +1996,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="5" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>156</v>
       </c>
@@ -965,7 +2014,7 @@
       </c>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>153</v>
       </c>
@@ -983,7 +2032,7 @@
       </c>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>155</v>
       </c>
@@ -1001,7 +2050,7 @@
       </c>
       <c r="G6" s="1"/>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>14</v>
       </c>
@@ -1015,7 +2064,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>156</v>
       </c>
@@ -1033,7 +2082,7 @@
       </c>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>156</v>
       </c>
@@ -1051,7 +2100,7 @@
       </c>
       <c r="G9" s="1"/>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>157</v>
       </c>
@@ -1069,7 +2118,7 @@
       </c>
       <c r="G10" s="1"/>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>157</v>
       </c>
@@ -1105,7 +2154,7 @@
       </c>
       <c r="G12" s="1"/>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="1" t="s">
         <v>22</v>
       </c>
@@ -1116,7 +2165,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="1" t="s">
         <v>24</v>
       </c>
@@ -1130,7 +2179,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
         <v>27</v>
       </c>
@@ -1144,7 +2193,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>158</v>
       </c>
@@ -1158,7 +2207,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>158</v>
       </c>
@@ -1176,7 +2225,7 @@
       </c>
       <c r="G17" s="1"/>
     </row>
-    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>153</v>
       </c>
@@ -1194,7 +2243,10 @@
       </c>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>88</v>
       </c>
@@ -1208,7 +2260,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>158</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>91</v>
       </c>
@@ -1222,7 +2277,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B21" s="1" t="s">
         <v>93</v>
       </c>
@@ -1239,7 +2294,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B22" s="1" t="s">
         <v>95</v>
       </c>
@@ -1253,7 +2308,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B23" s="1" t="s">
         <v>36</v>
       </c>
@@ -1351,7 +2406,7 @@
       </c>
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B28" s="1" t="s">
         <v>132</v>
       </c>
@@ -1365,7 +2420,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1379,7 +2434,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B30" s="1" t="s">
         <v>99</v>
       </c>
@@ -1393,7 +2448,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B31" s="1" t="s">
         <v>101</v>
       </c>
@@ -1407,7 +2462,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B32" s="1" t="s">
         <v>103</v>
       </c>
@@ -1421,7 +2476,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B33" s="1" t="s">
         <v>53</v>
       </c>
@@ -1477,7 +2532,7 @@
       </c>
       <c r="G35" s="1"/>
     </row>
-    <row r="36" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B36" s="1" t="s">
         <v>105</v>
       </c>
@@ -1494,7 +2549,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B37" s="1" t="s">
         <v>126</v>
       </c>
@@ -1508,7 +2563,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B38" s="1" t="s">
         <v>11</v>
       </c>
@@ -1525,7 +2580,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>161</v>
       </c>
@@ -1546,7 +2601,7 @@
       </c>
       <c r="G39" s="1"/>
     </row>
-    <row r="40" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>153</v>
       </c>
@@ -1567,7 +2622,7 @@
       </c>
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B41" s="1" t="s">
         <v>63</v>
       </c>
@@ -1584,7 +2639,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="42" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B42" s="1" t="s">
         <v>149</v>
       </c>
@@ -1598,7 +2653,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="43" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B43" s="1" t="s">
         <v>67</v>
       </c>
@@ -1615,7 +2670,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="44" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B44" s="1" t="s">
         <v>135</v>
       </c>
@@ -1632,7 +2687,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="45" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>158</v>
       </c>
@@ -1650,7 +2705,7 @@
       </c>
       <c r="G45" s="1"/>
     </row>
-    <row r="46" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>158</v>
       </c>
@@ -1668,7 +2723,7 @@
       </c>
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>158</v>
       </c>
@@ -1686,7 +2741,7 @@
       </c>
       <c r="G47" s="1"/>
     </row>
-    <row r="48" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>158</v>
       </c>
@@ -1704,7 +2759,7 @@
       </c>
       <c r="G48" s="1"/>
     </row>
-    <row r="49" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B49" s="1" t="s">
         <v>113</v>
       </c>
@@ -1721,7 +2776,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="50" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>157</v>
       </c>
@@ -1739,7 +2794,7 @@
       </c>
       <c r="G50" s="1"/>
     </row>
-    <row r="51" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>157</v>
       </c>
@@ -1757,7 +2812,7 @@
       </c>
       <c r="G51" s="1"/>
     </row>
-    <row r="52" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>157</v>
       </c>
@@ -1778,7 +2833,7 @@
       </c>
       <c r="G52" s="1"/>
     </row>
-    <row r="53" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>157</v>
       </c>
@@ -1796,17 +2851,10 @@
       </c>
       <c r="G53" s="1"/>
     </row>
-    <row r="54" spans="1:7" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B54" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I54" xr:uid="{6B0401B8-1E2A-4804-BB2B-70332DBFF9BB}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="ContainerCreator"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
More on Kubernetes API
</commit_message>
<xml_diff>
--- a/kubernetes/Kubernetes-API-Objects.xlsx
+++ b/kubernetes/Kubernetes-API-Objects.xlsx
@@ -1,17 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\dssg\Distributed-Systems-Study-Group\kubernetes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF417F84-3742-4593-BC16-B0D4DA9365CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041E85F3-8303-49CA-9FFC-D2D72D42C04B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6108" yWindow="3744" windowWidth="17280" windowHeight="8964" xr2:uid="{C9709F4E-DB8A-44C0-BA47-BF5BE7E9CD0A}"/>
-    <workbookView xWindow="6456" yWindow="4092" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{DC345DA8-84C6-4CD2-BFD8-497499F40304}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9709F4E-DB8A-44C0-BA47-BF5BE7E9CD0A}"/>
   </bookViews>
   <sheets>
     <sheet name="1.17" sheetId="8" r:id="rId1"/>
@@ -19,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'1.16'!$A$1:$I$54</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1.17'!$A$1:$I$54</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1.17'!$A$1:$I$57</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -922,10 +921,9 @@
   <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A52:A57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1937,9 +1935,6 @@
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="A12" sqref="A12"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>